<commit_message>
SEC-457 Final modifications for power tree board for release
</commit_message>
<xml_diff>
--- a/PCB design/01 - PowerTree/03 - DESIGN NOTES/BuckBoost_19V_DesignFile.xlsx
+++ b/PCB design/01 - PowerTree/03 - DESIGN NOTES/BuckBoost_19V_DesignFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\Projet\securbot\PCB design\01 - PowerTree\03 - DESIGN NOTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets\securbot\PCB design\01 - PowerTree\03 - DESIGN NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73FB3D-D6BC-435C-A1C3-DF31CB5581C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0570CAA6-6075-41E2-BE9B-43BACC926FC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8077ECEA-EE8E-4EA9-9E10-71A8436B8219}"/>
   </bookViews>
@@ -467,7 +467,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="##0.00E+0"/>
-    <numFmt numFmtId="166" formatCode="##0.0000E+0"/>
+    <numFmt numFmtId="165" formatCode="##0.0000E+0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -623,6 +623,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -632,7 +633,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -1968,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E200AC-79A8-4765-B18D-F7CE024EBD1C}">
   <dimension ref="A1:T231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,28 +1979,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="19"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2129,7 +2129,7 @@
       <c r="B26" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="16">
         <f>((C24/1.229)-1)*C25</f>
         <v>21689.585028478436</v>
       </c>

</xml_diff>